<commit_message>
thay doi sap xep bao cao
</commit_message>
<xml_diff>
--- a/public/excel/maunhapnguoilaodong.xlsx
+++ b/public/excel/maunhapnguoilaodong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E8BECE-4DC3-4529-B91C-5A209014BE74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA195DEF-C0E6-4F13-B38E-A3B8672303E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>29 Dương Văn An</t>
   </si>
   <si>
-    <t>Nữ</t>
-  </si>
-  <si>
     <t>Họ Tên</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>Column2</t>
   </si>
   <si>
-    <t>Nguyễn Du</t>
-  </si>
-  <si>
     <t>tenconty</t>
   </si>
   <si>
@@ -788,6 +782,12 @@
   </si>
   <si>
     <t>Cty A</t>
+  </si>
+  <si>
+    <t>Nguyễn Trọng Thuận</t>
+  </si>
+  <si>
+    <t>Nam</t>
   </si>
 </sst>
 </file>
@@ -2089,7 +2089,7 @@
   <dimension ref="A1:S272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,99 +2115,102 @@
   <sheetData>
     <row r="1" spans="1:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>6</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>11</v>
-      </c>
       <c r="L1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="N1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>63</v>
+        <v>252</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>253</v>
+      </c>
+      <c r="C2">
+        <v>999999999</v>
       </c>
       <c r="D2" s="1">
         <v>30853</v>
       </c>
       <c r="E2">
-        <v>4408400003</v>
+        <v>4408400005</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="N2" s="2">
         <f>VLOOKUP(I2,'Trình độ giáo dục'!$A$3:$B$6,2,0)</f>
@@ -2227,11 +2230,11 @@
       </c>
       <c r="R2" s="2">
         <f>VLOOKUP(M2,'công ty'!$A$3:$B$33,2,0)</f>
-        <v>3100994777</v>
+        <v>23451234521</v>
       </c>
       <c r="S2" s="2">
-        <f>VLOOKUP(G2,xã!$A$3:$B$153,2,0)</f>
-        <v>19</v>
+        <f>VLOOKUP(G2,xã!$A$2:$B$152,2,0)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -9533,7 +9536,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{CB5FE787-294C-47D4-B43C-3880200E545F}">
           <x14:formula1>
-            <xm:f>xã!$A$3:$A$153</xm:f>
+            <xm:f>xã!$A$2:$A$152</xm:f>
           </x14:formula1>
           <xm:sqref>G2</xm:sqref>
         </x14:dataValidation>
@@ -9583,8 +9586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65E91F1-C6C8-4E4E-8311-508FA1F9CF4D}">
   <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9595,15 +9598,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="10">
         <v>18</v>
@@ -9611,7 +9614,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="10">
         <v>19</v>
@@ -9619,7 +9622,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" s="10">
         <v>20</v>
@@ -9627,7 +9630,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="10">
         <v>21</v>
@@ -9635,7 +9638,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="10">
         <v>22</v>
@@ -9643,7 +9646,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="10">
         <v>23</v>
@@ -9651,7 +9654,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B8" s="10">
         <v>24</v>
@@ -9659,7 +9662,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="10">
         <v>25</v>
@@ -9667,7 +9670,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="10">
         <v>26</v>
@@ -9675,7 +9678,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="10">
         <v>27</v>
@@ -9683,7 +9686,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="10">
         <v>28</v>
@@ -9691,7 +9694,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" s="10">
         <v>29</v>
@@ -9699,7 +9702,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="10">
         <v>30</v>
@@ -9707,7 +9710,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B15" s="10">
         <v>31</v>
@@ -9715,7 +9718,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" s="10">
         <v>32</v>
@@ -9723,7 +9726,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B17" s="10">
         <v>33</v>
@@ -9731,7 +9734,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B18" s="10">
         <v>34</v>
@@ -9739,7 +9742,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" s="10">
         <v>35</v>
@@ -9747,7 +9750,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" s="10">
         <v>36</v>
@@ -9755,7 +9758,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" s="10">
         <v>37</v>
@@ -9763,7 +9766,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="10">
         <v>38</v>
@@ -9771,7 +9774,7 @@
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="10">
         <v>39</v>
@@ -9779,7 +9782,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" s="10">
         <v>40</v>
@@ -9787,7 +9790,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="10">
         <v>41</v>
@@ -9795,7 +9798,7 @@
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="10">
         <v>42</v>
@@ -9803,7 +9806,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" s="10">
         <v>43</v>
@@ -9811,7 +9814,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B28" s="10">
         <v>44</v>
@@ -9819,7 +9822,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B29" s="10">
         <v>45</v>
@@ -9827,7 +9830,7 @@
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B30" s="10">
         <v>46</v>
@@ -9835,7 +9838,7 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" s="10">
         <v>47</v>
@@ -9843,7 +9846,7 @@
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B32" s="10">
         <v>48</v>
@@ -9851,7 +9854,7 @@
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="10">
         <v>49</v>
@@ -9859,7 +9862,7 @@
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B34" s="10">
         <v>50</v>
@@ -9867,7 +9870,7 @@
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" s="10">
         <v>51</v>
@@ -9875,7 +9878,7 @@
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B36" s="10">
         <v>52</v>
@@ -9883,7 +9886,7 @@
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B37" s="10">
         <v>53</v>
@@ -9891,7 +9894,7 @@
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" s="10">
         <v>54</v>
@@ -9899,7 +9902,7 @@
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" s="10">
         <v>55</v>
@@ -9907,7 +9910,7 @@
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" s="10">
         <v>56</v>
@@ -9915,7 +9918,7 @@
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B41" s="10">
         <v>57</v>
@@ -9923,7 +9926,7 @@
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B42" s="10">
         <v>58</v>
@@ -9931,7 +9934,7 @@
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B43" s="10">
         <v>59</v>
@@ -9939,7 +9942,7 @@
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B44" s="10">
         <v>60</v>
@@ -9947,7 +9950,7 @@
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B45" s="10">
         <v>61</v>
@@ -9955,7 +9958,7 @@
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B46" s="10">
         <v>62</v>
@@ -9963,7 +9966,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B47" s="10">
         <v>63</v>
@@ -9971,7 +9974,7 @@
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B48" s="10">
         <v>64</v>
@@ -9979,7 +9982,7 @@
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B49" s="10">
         <v>65</v>
@@ -9987,7 +9990,7 @@
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B50" s="10">
         <v>66</v>
@@ -9995,7 +9998,7 @@
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B51" s="10">
         <v>67</v>
@@ -10003,7 +10006,7 @@
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B52" s="10">
         <v>68</v>
@@ -10011,7 +10014,7 @@
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B53" s="10">
         <v>69</v>
@@ -10019,7 +10022,7 @@
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B54" s="10">
         <v>70</v>
@@ -10027,7 +10030,7 @@
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B55" s="10">
         <v>71</v>
@@ -10035,7 +10038,7 @@
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B56" s="10">
         <v>72</v>
@@ -10043,7 +10046,7 @@
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B57" s="10">
         <v>73</v>
@@ -10051,7 +10054,7 @@
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" s="10">
         <v>74</v>
@@ -10059,7 +10062,7 @@
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B59" s="10">
         <v>75</v>
@@ -10067,7 +10070,7 @@
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B60" s="10">
         <v>76</v>
@@ -10075,7 +10078,7 @@
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B61" s="10">
         <v>77</v>
@@ -10083,7 +10086,7 @@
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B62" s="10">
         <v>78</v>
@@ -10091,7 +10094,7 @@
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B63" s="10">
         <v>79</v>
@@ -10099,7 +10102,7 @@
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B64" s="10">
         <v>80</v>
@@ -10107,7 +10110,7 @@
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B65" s="10">
         <v>81</v>
@@ -10115,7 +10118,7 @@
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" s="10">
         <v>82</v>
@@ -10123,7 +10126,7 @@
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B67" s="10">
         <v>83</v>
@@ -10131,7 +10134,7 @@
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B68" s="10">
         <v>84</v>
@@ -10139,7 +10142,7 @@
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B69" s="10">
         <v>85</v>
@@ -10147,7 +10150,7 @@
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B70" s="10">
         <v>86</v>
@@ -10155,7 +10158,7 @@
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B71" s="10">
         <v>87</v>
@@ -10163,7 +10166,7 @@
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" s="10">
         <v>88</v>
@@ -10171,7 +10174,7 @@
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B73" s="10">
         <v>89</v>
@@ -10179,7 +10182,7 @@
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B74" s="10">
         <v>90</v>
@@ -10187,7 +10190,7 @@
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B75" s="10">
         <v>91</v>
@@ -10195,7 +10198,7 @@
     </row>
     <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B76" s="10">
         <v>92</v>
@@ -10203,7 +10206,7 @@
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B77" s="10">
         <v>93</v>
@@ -10211,7 +10214,7 @@
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B78" s="10">
         <v>94</v>
@@ -10219,7 +10222,7 @@
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B79" s="10">
         <v>95</v>
@@ -10227,7 +10230,7 @@
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B80" s="10">
         <v>96</v>
@@ -10235,7 +10238,7 @@
     </row>
     <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B81" s="10">
         <v>97</v>
@@ -10243,7 +10246,7 @@
     </row>
     <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B82" s="10">
         <v>98</v>
@@ -10251,7 +10254,7 @@
     </row>
     <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B83" s="10">
         <v>99</v>
@@ -10259,7 +10262,7 @@
     </row>
     <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B84" s="10">
         <v>100</v>
@@ -10267,7 +10270,7 @@
     </row>
     <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B85" s="10">
         <v>101</v>
@@ -10275,7 +10278,7 @@
     </row>
     <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B86" s="10">
         <v>102</v>
@@ -10283,7 +10286,7 @@
     </row>
     <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B87" s="10">
         <v>103</v>
@@ -10291,7 +10294,7 @@
     </row>
     <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B88" s="10">
         <v>104</v>
@@ -10299,7 +10302,7 @@
     </row>
     <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B89" s="10">
         <v>105</v>
@@ -10307,7 +10310,7 @@
     </row>
     <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B90" s="10">
         <v>106</v>
@@ -10315,7 +10318,7 @@
     </row>
     <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B91" s="10">
         <v>107</v>
@@ -10323,7 +10326,7 @@
     </row>
     <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B92" s="10">
         <v>108</v>
@@ -10331,7 +10334,7 @@
     </row>
     <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B93" s="10">
         <v>109</v>
@@ -10339,7 +10342,7 @@
     </row>
     <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B94" s="10">
         <v>110</v>
@@ -10347,7 +10350,7 @@
     </row>
     <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B95" s="10">
         <v>111</v>
@@ -10355,7 +10358,7 @@
     </row>
     <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B96" s="10">
         <v>112</v>
@@ -10363,7 +10366,7 @@
     </row>
     <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B97" s="10">
         <v>113</v>
@@ -10371,7 +10374,7 @@
     </row>
     <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B98" s="10">
         <v>114</v>
@@ -10379,7 +10382,7 @@
     </row>
     <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B99" s="10">
         <v>115</v>
@@ -10387,7 +10390,7 @@
     </row>
     <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B100" s="10">
         <v>116</v>
@@ -10395,7 +10398,7 @@
     </row>
     <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B101" s="10">
         <v>117</v>
@@ -10403,7 +10406,7 @@
     </row>
     <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B102" s="10">
         <v>118</v>
@@ -10411,7 +10414,7 @@
     </row>
     <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B103" s="10">
         <v>119</v>
@@ -10419,7 +10422,7 @@
     </row>
     <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B104" s="10">
         <v>120</v>
@@ -10427,7 +10430,7 @@
     </row>
     <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B105" s="10">
         <v>121</v>
@@ -10435,7 +10438,7 @@
     </row>
     <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B106" s="10">
         <v>122</v>
@@ -10443,7 +10446,7 @@
     </row>
     <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B107" s="10">
         <v>123</v>
@@ -10451,7 +10454,7 @@
     </row>
     <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B108" s="10">
         <v>124</v>
@@ -10459,7 +10462,7 @@
     </row>
     <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B109" s="10">
         <v>125</v>
@@ -10467,7 +10470,7 @@
     </row>
     <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B110" s="10">
         <v>126</v>
@@ -10475,7 +10478,7 @@
     </row>
     <row r="111" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B111" s="10">
         <v>127</v>
@@ -10483,7 +10486,7 @@
     </row>
     <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B112" s="10">
         <v>128</v>
@@ -10491,7 +10494,7 @@
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B113" s="10">
         <v>129</v>
@@ -10499,7 +10502,7 @@
     </row>
     <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B114" s="10">
         <v>130</v>
@@ -10507,7 +10510,7 @@
     </row>
     <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B115" s="10">
         <v>131</v>
@@ -10515,7 +10518,7 @@
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B116" s="10">
         <v>132</v>
@@ -10523,7 +10526,7 @@
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B117" s="10">
         <v>133</v>
@@ -10531,7 +10534,7 @@
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B118" s="10">
         <v>134</v>
@@ -10539,7 +10542,7 @@
     </row>
     <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B119" s="10">
         <v>135</v>
@@ -10547,7 +10550,7 @@
     </row>
     <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B120" s="10">
         <v>136</v>
@@ -10555,7 +10558,7 @@
     </row>
     <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B121" s="10">
         <v>137</v>
@@ -10563,7 +10566,7 @@
     </row>
     <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B122" s="10">
         <v>138</v>
@@ -10571,7 +10574,7 @@
     </row>
     <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B123" s="10">
         <v>139</v>
@@ -10579,7 +10582,7 @@
     </row>
     <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B124" s="10">
         <v>140</v>
@@ -10587,7 +10590,7 @@
     </row>
     <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B125" s="10">
         <v>141</v>
@@ -10595,7 +10598,7 @@
     </row>
     <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B126" s="10">
         <v>142</v>
@@ -10603,7 +10606,7 @@
     </row>
     <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B127" s="10">
         <v>143</v>
@@ -10611,7 +10614,7 @@
     </row>
     <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B128" s="10">
         <v>144</v>
@@ -10619,7 +10622,7 @@
     </row>
     <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B129" s="10">
         <v>145</v>
@@ -10627,7 +10630,7 @@
     </row>
     <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B130" s="10">
         <v>146</v>
@@ -10635,7 +10638,7 @@
     </row>
     <row r="131" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B131" s="10">
         <v>147</v>
@@ -10643,7 +10646,7 @@
     </row>
     <row r="132" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B132" s="10">
         <v>148</v>
@@ -10651,7 +10654,7 @@
     </row>
     <row r="133" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B133" s="10">
         <v>149</v>
@@ -10659,7 +10662,7 @@
     </row>
     <row r="134" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B134" s="10">
         <v>150</v>
@@ -10667,7 +10670,7 @@
     </row>
     <row r="135" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B135" s="10">
         <v>151</v>
@@ -10675,7 +10678,7 @@
     </row>
     <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B136" s="10">
         <v>152</v>
@@ -10683,7 +10686,7 @@
     </row>
     <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B137" s="10">
         <v>153</v>
@@ -10691,7 +10694,7 @@
     </row>
     <row r="138" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B138" s="10">
         <v>154</v>
@@ -10699,7 +10702,7 @@
     </row>
     <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B139" s="10">
         <v>155</v>
@@ -10707,7 +10710,7 @@
     </row>
     <row r="140" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B140" s="10">
         <v>156</v>
@@ -10715,7 +10718,7 @@
     </row>
     <row r="141" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B141" s="10">
         <v>157</v>
@@ -10723,7 +10726,7 @@
     </row>
     <row r="142" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B142" s="10">
         <v>158</v>
@@ -10731,7 +10734,7 @@
     </row>
     <row r="143" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B143" s="10">
         <v>159</v>
@@ -10739,7 +10742,7 @@
     </row>
     <row r="144" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B144" s="10">
         <v>160</v>
@@ -10747,7 +10750,7 @@
     </row>
     <row r="145" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B145" s="10">
         <v>161</v>
@@ -10755,7 +10758,7 @@
     </row>
     <row r="146" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B146" s="10">
         <v>162</v>
@@ -10763,7 +10766,7 @@
     </row>
     <row r="147" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B147" s="10">
         <v>163</v>
@@ -10771,7 +10774,7 @@
     </row>
     <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B148" s="10">
         <v>164</v>
@@ -10779,7 +10782,7 @@
     </row>
     <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B149" s="10">
         <v>165</v>
@@ -10787,7 +10790,7 @@
     </row>
     <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B150" s="10">
         <v>166</v>
@@ -10795,7 +10798,7 @@
     </row>
     <row r="151" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B151" s="10">
         <v>167</v>
@@ -10803,7 +10806,7 @@
     </row>
     <row r="152" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B152" s="10">
         <v>168</v>
@@ -10811,7 +10814,7 @@
     </row>
     <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B153" s="6">
         <v>19108</v>
@@ -10842,23 +10845,23 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B3" s="10">
         <v>3100305441</v>
@@ -10866,7 +10869,7 @@
     </row>
     <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B4" s="10">
         <v>3101031264</v>
@@ -10874,7 +10877,7 @@
     </row>
     <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B5" s="10">
         <v>3101055473</v>
@@ -10882,7 +10885,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B6" s="10">
         <v>3100961669</v>
@@ -10890,7 +10893,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B7" s="10">
         <v>3100301817</v>
@@ -10898,7 +10901,7 @@
     </row>
     <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B8" s="10">
         <v>3100983214</v>
@@ -10906,7 +10909,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B9" s="10">
         <v>3101092651</v>
@@ -10914,7 +10917,7 @@
     </row>
     <row r="10" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B10" s="10">
         <v>3100300690</v>
@@ -10922,7 +10925,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B11" s="10">
         <v>3101068560</v>
@@ -10930,7 +10933,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B12" s="10">
         <v>3100287714</v>
@@ -10938,7 +10941,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B13" s="10">
         <v>3100386377</v>
@@ -10946,7 +10949,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B14" s="10">
         <v>3100193343</v>
@@ -10954,7 +10957,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B15" s="10">
         <v>3101100447</v>
@@ -10962,7 +10965,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B16" s="10">
         <v>3101082325</v>
@@ -10970,7 +10973,7 @@
     </row>
     <row r="17" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B17" s="10">
         <v>3101091601</v>
@@ -10978,7 +10981,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B18" s="10">
         <v>3100994777</v>
@@ -10986,7 +10989,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B19" s="10">
         <v>3100988357</v>
@@ -10994,7 +10997,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B20" s="10">
         <v>3100262413</v>
@@ -11002,7 +11005,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B21" s="10">
         <v>3100317380</v>
@@ -11010,7 +11013,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B22" s="10">
         <v>3100262452</v>
@@ -11018,7 +11021,7 @@
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B23" s="10">
         <v>3100382654</v>
@@ -11026,7 +11029,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B24" s="10">
         <v>3100301599</v>
@@ -11034,7 +11037,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B25" s="10">
         <v>3101051292</v>
@@ -11042,7 +11045,7 @@
     </row>
     <row r="26" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B26" s="10">
         <v>3100733422</v>
@@ -11050,7 +11053,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B27" s="10">
         <v>3101001076</v>
@@ -11058,7 +11061,7 @@
     </row>
     <row r="28" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B28" s="10">
         <v>3100385782</v>
@@ -11066,7 +11069,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B29" s="10">
         <v>3100485755</v>
@@ -11074,7 +11077,7 @@
     </row>
     <row r="30" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B30" s="10">
         <v>3101069155</v>
@@ -11082,7 +11085,7 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B31" s="10">
         <v>3100996083</v>
@@ -11090,7 +11093,7 @@
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B32" s="10">
         <v>3100954157</v>
@@ -11098,7 +11101,7 @@
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B33" s="7">
         <v>23451234521</v>
@@ -11128,23 +11131,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2">
         <v>20221108050440</v>
@@ -11152,7 +11155,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2">
         <v>20221108050455</v>
@@ -11160,7 +11163,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2">
         <v>20221108050508</v>
@@ -11190,23 +11193,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -11214,7 +11217,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -11222,7 +11225,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -11230,7 +11233,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -11238,7 +11241,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -11246,7 +11249,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -11254,7 +11257,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -11262,7 +11265,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -11270,7 +11273,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -11278,7 +11281,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -11286,7 +11289,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -11294,7 +11297,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -11302,7 +11305,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -11310,7 +11313,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -11318,7 +11321,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -11326,7 +11329,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -11334,7 +11337,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -11342,7 +11345,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -11350,7 +11353,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -11358,7 +11361,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -11366,7 +11369,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -11374,7 +11377,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -11382,7 +11385,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -11412,23 +11415,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2">
         <v>20221108050223</v>
@@ -11436,7 +11439,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>20221108050239</v>
@@ -11444,7 +11447,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2">
         <v>20221108050251</v>
@@ -11452,7 +11455,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2">
         <v>20221108050306</v>
@@ -11460,7 +11463,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2">
         <v>20221108050317</v>
@@ -11468,7 +11471,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2">
         <v>20221108050331</v>
@@ -11476,7 +11479,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2">
         <v>20221108050342</v>
@@ -11484,7 +11487,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>20221108050354</v>
@@ -11514,23 +11517,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>20221108050055</v>
@@ -11538,7 +11541,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>20221108050124</v>
@@ -11546,7 +11549,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>20221108050141</v>
@@ -11554,7 +11557,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>20221108050156</v>

</xml_diff>